<commit_message>
Se agregan 6 archivos de carga de imagenes
</commit_message>
<xml_diff>
--- a/csv/Mario.xlsx
+++ b/csv/Mario.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12375"/>
+    <workbookView windowWidth="28800" windowHeight="12375" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="0-config.csv" sheetId="2" r:id="rId1"/>
@@ -15,7 +15,7 @@
     <sheet name="5-boots.csv" sheetId="6" r:id="rId6"/>
     <sheet name="carga.csv" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="144525" iterate="1" iterateCount="100" iterateDelta="0.001"/>
 </workbook>
 </file>
 
@@ -90,10 +90,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -132,16 +132,16 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -156,7 +156,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -164,59 +164,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -237,9 +185,62 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -253,15 +254,14 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="40">
+  <fills count="39">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -294,12 +294,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF86592D"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="1"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -318,61 +312,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -390,7 +336,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -402,73 +408,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -486,13 +432,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -503,6 +497,15 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -538,48 +541,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -603,12 +564,45 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -632,128 +626,128 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="32" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -775,10 +769,7 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1112,7 +1103,7 @@
   <sheetPr/>
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -1242,28 +1233,28 @@
       <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="K2" s="8" t="s">
+      <c r="D2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" s="7" t="s">
         <v>7</v>
       </c>
       <c r="L2" t="s">
@@ -1292,28 +1283,28 @@
       <c r="C3" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="K3" s="8" t="s">
+      <c r="D3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="K3" s="7" t="s">
         <v>7</v>
       </c>
       <c r="L3" t="s">
@@ -1339,37 +1330,37 @@
       <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="I4" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="J4" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="K4" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="L4" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="M4" s="8" t="s">
+      <c r="C4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="L4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="M4" s="7" t="s">
         <v>7</v>
       </c>
       <c r="N4" t="s">
@@ -1389,40 +1380,40 @@
       <c r="B5" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="I5" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="J5" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="K5" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="L5" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="M5" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="N5" s="8" t="s">
+      <c r="C5" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="L5" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="M5" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="N5" s="7" t="s">
         <v>7</v>
       </c>
       <c r="O5" t="s">
@@ -1439,37 +1430,37 @@
       <c r="B6" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="I6" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="J6" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="K6" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="L6" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="M6" s="8" t="s">
+      <c r="C6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="L6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="M6" s="7" t="s">
         <v>7</v>
       </c>
       <c r="N6" t="s">
@@ -1495,28 +1486,28 @@
       <c r="D7" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="H7" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="I7" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="J7" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="K7" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="L7" s="8" t="s">
+      <c r="E7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="L7" s="7" t="s">
         <v>7</v>
       </c>
       <c r="M7" t="s">
@@ -1542,25 +1533,25 @@
       <c r="C8" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="G8" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="H8" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="I8" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="J8" s="8" t="s">
+      <c r="D8" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J8" s="7" t="s">
         <v>7</v>
       </c>
       <c r="K8" t="s">
@@ -1589,37 +1580,37 @@
       <c r="B9" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="G9" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="H9" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="I9" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="J9" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="K9" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="L9" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="M9" s="8" t="s">
+      <c r="C9" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="L9" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="M9" s="7" t="s">
         <v>7</v>
       </c>
       <c r="N9" t="s">
@@ -1636,40 +1627,40 @@
       <c r="A10" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="H10" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="I10" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="J10" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="K10" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="L10" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="M10" s="8" t="s">
+      <c r="B10" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J10" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="K10" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="L10" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="M10" s="7" t="s">
         <v>7</v>
       </c>
       <c r="N10" t="s">
@@ -1686,40 +1677,40 @@
       <c r="A11" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="H11" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="I11" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="J11" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="K11" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="L11" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="M11" s="8" t="s">
+      <c r="B11" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J11" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="K11" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="L11" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="M11" s="7" t="s">
         <v>7</v>
       </c>
       <c r="N11" t="s">
@@ -1736,40 +1727,40 @@
       <c r="A12" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="H12" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="I12" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="J12" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="K12" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="L12" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="M12" s="8" t="s">
+      <c r="B12" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J12" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="K12" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="L12" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="M12" s="7" t="s">
         <v>7</v>
       </c>
       <c r="N12" t="s">
@@ -1786,40 +1777,40 @@
       <c r="A13" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F13" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="G13" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="H13" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="I13" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="J13" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="K13" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="L13" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="M13" s="8" t="s">
+      <c r="B13" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I13" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J13" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="K13" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="L13" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="M13" s="7" t="s">
         <v>7</v>
       </c>
       <c r="N13" t="s">
@@ -1842,13 +1833,13 @@
       <c r="C14" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F14" s="8" t="s">
+      <c r="D14" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14" s="7" t="s">
         <v>7</v>
       </c>
       <c r="G14" t="s">
@@ -1857,13 +1848,13 @@
       <c r="H14" t="s">
         <v>6</v>
       </c>
-      <c r="I14" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="J14" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="K14" s="8" t="s">
+      <c r="I14" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J14" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="K14" s="7" t="s">
         <v>7</v>
       </c>
       <c r="L14" t="s">
@@ -1889,13 +1880,13 @@
       <c r="B15" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E15" s="8" t="s">
+      <c r="C15" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" s="7" t="s">
         <v>7</v>
       </c>
       <c r="F15" t="s">
@@ -1910,13 +1901,13 @@
       <c r="I15" t="s">
         <v>6</v>
       </c>
-      <c r="J15" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="K15" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="L15" s="8" t="s">
+      <c r="J15" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="K15" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="L15" s="7" t="s">
         <v>7</v>
       </c>
       <c r="M15" t="s">
@@ -1936,16 +1927,16 @@
       <c r="A16" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E16" s="8" t="s">
+      <c r="B16" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="7" t="s">
         <v>7</v>
       </c>
       <c r="F16" t="s">
@@ -1960,16 +1951,16 @@
       <c r="I16" t="s">
         <v>6</v>
       </c>
-      <c r="J16" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="K16" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="L16" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="M16" s="8" t="s">
+      <c r="J16" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="K16" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="L16" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="M16" s="7" t="s">
         <v>7</v>
       </c>
       <c r="N16" t="s">
@@ -2115,10 +2106,10 @@
       <c r="D3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G3" t="s">
@@ -2130,7 +2121,7 @@
       <c r="I3" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="7" t="s">
+      <c r="J3" s="6" t="s">
         <v>10</v>
       </c>
       <c r="K3" t="s">
@@ -2180,7 +2171,7 @@
       <c r="I4" t="s">
         <v>6</v>
       </c>
-      <c r="J4" s="7" t="s">
+      <c r="J4" s="6" t="s">
         <v>10</v>
       </c>
       <c r="K4" t="s">
@@ -2233,7 +2224,7 @@
       <c r="J5" t="s">
         <v>6</v>
       </c>
-      <c r="K5" s="7" t="s">
+      <c r="K5" s="6" t="s">
         <v>10</v>
       </c>
       <c r="L5" t="s">
@@ -2280,16 +2271,16 @@
       <c r="I6" t="s">
         <v>6</v>
       </c>
-      <c r="J6" s="7" t="s">
+      <c r="J6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="K6" s="7" t="s">
+      <c r="K6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="L6" s="7" t="s">
+      <c r="L6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="M6" s="7" t="s">
+      <c r="M6" s="6" t="s">
         <v>10</v>
       </c>
       <c r="N6" t="s">
@@ -5273,11 +5264,14 @@
   <sheetPr/>
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="A1:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="6" outlineLevelCol="1"/>
+  <cols>
+    <col min="2" max="2" width="15.4285714285714" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">

</xml_diff>